<commit_message>
Corrección de numero de partes en PCB_A
</commit_message>
<xml_diff>
--- a/Hardware/Satelite/PCB_A/BOM.xlsx
+++ b/Hardware/Satelite/PCB_A/BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="93">
   <si>
     <t>Component</t>
   </si>
@@ -51,9 +51,6 @@
     <t>C_Small</t>
   </si>
   <si>
-    <t>C4 C5 C6 C9 C10 C11 C12</t>
-  </si>
-  <si>
     <t>100nF</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t>GCM155R71C104KA55D</t>
   </si>
   <si>
-    <t>C2</t>
-  </si>
-  <si>
     <t>C_0603_1608Metric_Pad1.05x0.95mm_HandSolder</t>
   </si>
   <si>
@@ -292,6 +286,18 @@
   </si>
   <si>
     <t>LMK107B7105MA-T</t>
+  </si>
+  <si>
+    <t>C2 C4 C5 C6 C9 C10 C11 C12</t>
+  </si>
+  <si>
+    <t>22-28-5034</t>
+  </si>
+  <si>
+    <t>22-28-4041</t>
+  </si>
+  <si>
+    <t>150060VS75000</t>
   </si>
 </sst>
 </file>
@@ -844,8 +850,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:H24" totalsRowShown="0">
-  <autoFilter ref="A1:H24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:H23" totalsRowShown="0">
+  <autoFilter ref="A1:H23"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Component"/>
     <tableColumn id="2" name="Description"/>
@@ -1123,10 +1129,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1135,7 +1141,7 @@
     <col min="2" max="2" width="22.69140625" customWidth="1"/>
     <col min="4" max="4" width="11.765625" customWidth="1"/>
     <col min="5" max="5" width="17.53515625" customWidth="1"/>
-    <col min="6" max="6" width="19.15234375" customWidth="1"/>
+    <col min="6" max="6" width="48.4609375" customWidth="1"/>
     <col min="7" max="7" width="16.69140625" customWidth="1"/>
     <col min="8" max="8" width="40.3828125" style="2" customWidth="1"/>
   </cols>
@@ -1177,19 +1183,19 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="G2">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.4">
@@ -1206,16 +1212,16 @@
         <v>14</v>
       </c>
       <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
@@ -1229,19 +1235,19 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>18</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
@@ -1249,85 +1255,82 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
         <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" t="s">
-        <v>25</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
         <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>30</v>
@@ -1342,73 +1345,76 @@
         <v>30</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G9">
-        <v>3</v>
-      </c>
-      <c r="H9" s="2">
-        <v>61300311121</v>
+        <v>2</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10" s="2">
-        <v>61300411121</v>
+        <v>61300311121</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
         <v>36</v>
-      </c>
-      <c r="E11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" t="s">
-        <v>38</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -1419,74 +1425,74 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G12">
         <v>1</v>
       </c>
-      <c r="H12" s="2">
-        <v>61300311121</v>
+      <c r="H12" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F13" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>50</v>
@@ -1494,126 +1500,126 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E15" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F15" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F16" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" t="s">
         <v>61</v>
       </c>
-      <c r="E17" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" t="s">
-        <v>63</v>
-      </c>
       <c r="G17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F18" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A19">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="D19" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E19" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F19" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1624,136 +1630,110 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A20">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" t="s">
         <v>73</v>
       </c>
-      <c r="E20" t="s">
-        <v>72</v>
-      </c>
       <c r="F20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A21">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" t="s">
         <v>76</v>
       </c>
-      <c r="E21" t="s">
-        <v>75</v>
-      </c>
       <c r="F21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A22">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C22" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D22" t="s">
+        <v>80</v>
+      </c>
+      <c r="E22" t="s">
         <v>79</v>
       </c>
-      <c r="E22" t="s">
-        <v>78</v>
-      </c>
       <c r="F22" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G22">
         <v>1</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D23" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E23" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F23" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G23">
         <v>1</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A24">
-        <v>26</v>
-      </c>
-      <c r="B24" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24" t="s">
-        <v>85</v>
-      </c>
-      <c r="D24" t="s">
-        <v>86</v>
-      </c>
-      <c r="E24" t="s">
         <v>87</v>
       </c>
-      <c r="F24" t="s">
-        <v>88</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B37" s="1"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B36" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>